<commit_message>
update 1;10 pm 19/6 from PC
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/PHP.xlsx
+++ b/PHP-Course/BackEnd-PHP/PHP.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PHP" sheetId="3" r:id="rId1"/>
     <sheet name="Toán tử" sheetId="4" r:id="rId2"/>
     <sheet name="Form" sheetId="5" r:id="rId3"/>
     <sheet name="Câu điều kiện" sheetId="6" r:id="rId4"/>
-    <sheet name="Vòng Lặp" sheetId="7" r:id="rId5"/>
+    <sheet name="Câu DK SWiTCH" sheetId="8" r:id="rId5"/>
+    <sheet name="Vòng Lặp" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="203">
   <si>
     <t>*</t>
   </si>
@@ -543,9 +544,6 @@
     <t>$result = "Số lẻ";</t>
   </si>
   <si>
-    <t>$result = "Số chẵn";</t>
-  </si>
-  <si>
     <t>$number = -7;</t>
   </si>
   <si>
@@ -646,6 +644,119 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">If … 
+Else If 
+… Else </t>
+  </si>
+  <si>
+    <t>$number = 0;</t>
+  </si>
+  <si>
+    <t>$n = $number % 2;</t>
+  </si>
+  <si>
+    <t>$resultFirst = ($number &gt;= 0) ? "Nguyên dương" : "Nguyên âm";</t>
+  </si>
+  <si>
+    <t>$resultLast = ($n == 0) ? "chẵn" :  "lẻ";</t>
+  </si>
+  <si>
+    <t>$result = $resultFirst . " " . $resultLast;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If … 
+Else If 
+… Else
+Rút gọn </t>
+  </si>
+  <si>
+    <t>Có 1 đk mặc định, nghĩa là khi giá trị đưa vào không thỏa mãn 1 đk nào đó 
+thì nó sẽ lấy các câu lệnh trong phần đk mặc định để thực hiện</t>
+  </si>
+  <si>
+    <t>Các vòng lặp thường sử dụng trong PHP</t>
+  </si>
+  <si>
+    <t>For</t>
+  </si>
+  <si>
+    <t>While</t>
+  </si>
+  <si>
+    <t>Do … While</t>
+  </si>
+  <si>
+    <t>For … Each</t>
+  </si>
+  <si>
+    <t>METHOD</t>
+  </si>
+  <si>
+    <t>Cách thức dữ liệu được gửi đi ( POST or GET )</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>xác định trang/tập tin các dữ liệu được gửi đến để xủ lý chúng</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Tên của form</t>
+  </si>
+  <si>
+    <t>href : Tên địa chỉ trang web hiện ra</t>
+  </si>
+  <si>
+    <t>isset () : Kiểm tra biến có tồn tại hay không ?</t>
+  </si>
+  <si>
+    <r>
+      <t>echo $_POST["</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"] . "&lt;br/&gt;";</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>echo $_POST["</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"];</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -661,82 +772,53 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t> ($number % 2 == 0) {</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">If … 
-Else If 
-… Else </t>
-  </si>
-  <si>
-    <t>$number = 0;</t>
-  </si>
-  <si>
-    <t>$n = $number % 2;</t>
-  </si>
-  <si>
-    <t>$resultFirst = ($number &gt;= 0) ? "Nguyên dương" : "Nguyên âm";</t>
-  </si>
-  <si>
-    <t>$resultLast = ($n == 0) ? "chẵn" :  "lẻ";</t>
-  </si>
-  <si>
-    <t>$result = $resultFirst . " " . $resultLast;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If … 
-Else If 
-… Else
-Rút gọn </t>
-  </si>
-  <si>
-    <t>Có 1 đk mặc định, nghĩa là khi giá trị đưa vào không thỏa mãn 1 đk nào đó 
-thì nó sẽ lấy các câu lệnh trong phần đk mặc định để thực hiện</t>
-  </si>
-  <si>
-    <t>Các vòng lặp thường sử dụng trong PHP</t>
-  </si>
-  <si>
-    <t>For</t>
-  </si>
-  <si>
-    <t>While</t>
-  </si>
-  <si>
-    <t>Do … While</t>
-  </si>
-  <si>
-    <t>For … Each</t>
-  </si>
-  <si>
-    <t>METHOD</t>
-  </si>
-  <si>
-    <t>Cách thức dữ liệu được gửi đi ( POST or GET )</t>
-  </si>
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>xác định trang/tập tin các dữ liệu được gửi đến để xủ lý chúng</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>Tên của form</t>
-  </si>
-  <si>
-    <t>href : Tên địa chỉ trang web hiện ra</t>
-  </si>
-  <si>
-    <t>isset () : Kiểm tra biến có tồn tại hay không ?</t>
-  </si>
-  <si>
-    <r>
-      <t>echo $_POST["</t>
-    </r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$number % 2 == 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$result = "Số chẵn"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>isset ($_POST["number1"]) == true</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -744,7 +826,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>email</t>
+      <t>if</t>
     </r>
     <r>
       <rPr>
@@ -752,12 +834,112 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>"] . "&lt;br/&gt;";</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>echo $_POST["</t>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$number % 2 == 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <t>if () {}</t>
+  </si>
+  <si>
+    <t>if () {} else {}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if () {} elseif () {}
+         elseif () {}
+         else {}
+</t>
+  </si>
+  <si>
+    <t>Rút gọn</t>
+  </si>
+  <si>
+    <t>isset ($_POST["number1"])</t>
+  </si>
+  <si>
+    <t>&lt;?php</t>
+  </si>
+  <si>
+    <t>         </t>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <t>        $n1     = "";</t>
+  </si>
+  <si>
+    <t>        $n2     = "";</t>
+  </si>
+  <si>
+    <t>        $caculate     = "";</t>
+  </si>
+  <si>
+    <t>        if (isset ($_POST["number1"]) == true &amp;&amp; </t>
+  </si>
+  <si>
+    <t>            isset ($_POST["number2"]) == true &amp;&amp; </t>
+  </si>
+  <si>
+    <t>            isset ($_POST["caculate"]) == true ) {</t>
+  </si>
+  <si>
+    <t>                echo $n1     = $_POST["number1"];</t>
+  </si>
+  <si>
+    <t>                echo $n2     = $_POST["number2"]; </t>
+  </si>
+  <si>
+    <t>                echo $caculate     = $_POST["caculate"];   </t>
+  </si>
+  <si>
+    <t>    ?&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;input type="text" name="number1" </t>
     </r>
     <r>
       <rPr>
@@ -766,7 +948,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>password</t>
+      <t>value="&lt;?php echo $n1; ?&gt;"</t>
     </r>
     <r>
       <rPr>
@@ -774,15 +956,21 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>"];</t>
-    </r>
+      <t> /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Đặt tên biến đầu tiên</t>
+  </si>
+  <si>
+    <t>Để giữ lại giá trị của ô input khi người dùng đã nhập xong dữ liệu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -835,6 +1023,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -844,7 +1038,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -867,12 +1061,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,6 +1184,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -938,6 +1197,42 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1982,12 +2277,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="7" t="s">
         <v>41</v>
       </c>
@@ -1996,34 +2291,34 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="7" t="s">
         <v>41</v>
       </c>
@@ -2033,10 +2328,10 @@
       <c r="F30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="23"/>
+      <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
@@ -2076,21 +2371,21 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="22"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="15" t="s">
         <v>41</v>
       </c>
@@ -2198,10 +2493,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,28 +2536,28 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2293,7 +2588,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2301,7 +2596,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -2312,7 +2607,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -2320,10 +2615,10 @@
         <v>130</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -2331,17 +2626,33 @@
         <v>132</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>177</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I25" t="s">
+        <v>185</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2357,10 +2668,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,195 +2717,242 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>143</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="26"/>
+      <c r="L8" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="3" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K7" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="L7" s="3" t="s">
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K10" s="26"/>
+      <c r="L10" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="22"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="3"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="22"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="3"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="26"/>
+      <c r="F15" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="25"/>
-      <c r="F12" s="3" t="s">
+      <c r="K16" s="26"/>
+      <c r="L16" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="3" t="s">
+      <c r="K17" s="26"/>
+      <c r="L17" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="3" t="s">
+      <c r="K18" s="26"/>
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="22"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="21"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K16" s="25"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B21:J22"/>
-    <mergeCell ref="A13:A19"/>
+  <mergeCells count="6">
+    <mergeCell ref="B26:J27"/>
+    <mergeCell ref="A16:A22"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="E7:E17"/>
-    <mergeCell ref="K7:K17"/>
+    <mergeCell ref="E7:E20"/>
+    <mergeCell ref="K7:K20"/>
+    <mergeCell ref="F22:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2602,6 +2960,170 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+    </row>
+    <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="36"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I20" s="38"/>
+      <c r="J20" s="39"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="I2:J20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2619,27 +3141,27 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update - File excel PHP (Hàm) & VS Code (Hàm) 3:21 PM 20/06/2020
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/PHP.xlsx
+++ b/PHP-Course/BackEnd-PHP/PHP.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="PHP" sheetId="3" r:id="rId1"/>
@@ -12,9 +12,13 @@
     <sheet name="Form" sheetId="5" r:id="rId3"/>
     <sheet name="Câu điều kiện" sheetId="6" r:id="rId4"/>
     <sheet name="Câu DK SWiTCH" sheetId="8" r:id="rId5"/>
-    <sheet name="Vòng Lặp" sheetId="7" r:id="rId6"/>
+    <sheet name="BT Câu ĐK" sheetId="9" r:id="rId6"/>
+    <sheet name="Vòng Lặp" sheetId="7" r:id="rId7"/>
+    <sheet name="Hàm 1" sheetId="10" r:id="rId8"/>
+    <sheet name="Hàm 2" sheetId="11" r:id="rId9"/>
+    <sheet name="Hàm 3" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -24,7 +28,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D19" authorId="0" shapeId="0">
+    <comment ref="D19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,8 +80,32 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="J32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gọi Hàm createBox() ra</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="381">
   <si>
     <t>*</t>
   </si>
@@ -960,10 +988,1046 @@
     </r>
   </si>
   <si>
-    <t>Đặt tên biến đầu tiên</t>
-  </si>
-  <si>
     <t>Để giữ lại giá trị của ô input khi người dùng đã nhập xong dữ liệu</t>
+  </si>
+  <si>
+    <t>        </t>
+  </si>
+  <si>
+    <t>            }</t>
+  </si>
+  <si>
+    <t>    }</t>
+  </si>
+  <si>
+    <t>?&gt;</t>
+  </si>
+  <si>
+    <t>                        }</t>
+  </si>
+  <si>
+    <t>$n1                = "";</t>
+  </si>
+  <si>
+    <t>    $n2             = "";</t>
+  </si>
+  <si>
+    <t>    $caculate       = "";</t>
+  </si>
+  <si>
+    <t>    if(isset($_POST["number1"]) &amp;&amp; isset($_POST["number2"]) &amp;&amp; isset($_POST["caculate"])){</t>
+  </si>
+  <si>
+    <t>        $n1         = $_POST["number1"];</t>
+  </si>
+  <si>
+    <t>        $n2         = $_POST["number2"];</t>
+  </si>
+  <si>
+    <t>        $caculate   = $_POST["caculate"];</t>
+  </si>
+  <si>
+    <t>        $flag       = true;</t>
+  </si>
+  <si>
+    <t>        if(is_numeric($n1) &amp;&amp; is_numeric($n2) ){</t>
+  </si>
+  <si>
+    <t>            switch ($caculate) {</t>
+  </si>
+  <si>
+    <t>                case "+":</t>
+  </si>
+  <si>
+    <t>                    $result = $n1 + $n2;</t>
+  </si>
+  <si>
+    <t>                    break;</t>
+  </si>
+  <si>
+    <t>                case "-":</t>
+  </si>
+  <si>
+    <t>                    $result = $n1 - $n2;</t>
+  </si>
+  <si>
+    <t>                case "*":</t>
+  </si>
+  <si>
+    <t>                case "x":</t>
+  </si>
+  <si>
+    <t>                    $result = $n1 * $n2;</t>
+  </si>
+  <si>
+    <t>                case "/":</t>
+  </si>
+  <si>
+    <t>                case ":":</t>
+  </si>
+  <si>
+    <t>                    $result = $n1 / $n2;</t>
+  </si>
+  <si>
+    <t>                case "%":</t>
+  </si>
+  <si>
+    <t>                    $result = $n1 % $n2;</t>
+  </si>
+  <si>
+    <t>                default:</t>
+  </si>
+  <si>
+    <t>                    $caculate = "+";</t>
+  </si>
+  <si>
+    <t>        } else {</t>
+  </si>
+  <si>
+    <t>            $result = "Không thực hiện được";</t>
+  </si>
+  <si>
+    <t>            $flag   = false;</t>
+  </si>
+  <si>
+    <t>    &lt;div class="content"&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;h1&gt;Mô phỏng máy tính điện tử&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;form action="#" method="post" name="main-form"&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;div class="row"&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;span&gt;Số thứ nhất&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;input type="text" name="number1" value="&lt;?php echo $n1;?&gt;"/&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;span&gt;Phép toán&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;input type="text" name="caculate" value="&lt;?php echo $caculate;?&gt;"/&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;span&gt;Số thứ hai&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;input type="text" name="number2" value="&lt;?php echo $n2;?&gt;"/&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;input type="submit" value="Xem kết quả" name="submit"/&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;p&gt;</t>
+  </si>
+  <si>
+    <t>                    &lt;?php </t>
+  </si>
+  <si>
+    <t>                            echo "Kết quả " . $n1 . " " . $caculate . " " . $n2 . " = " . $result;</t>
+  </si>
+  <si>
+    <t>                        } else {</t>
+  </si>
+  <si>
+    <t>                            echo $result;</t>
+  </si>
+  <si>
+    <r>
+      <t>                        if(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$flag==true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>){</t>
+    </r>
+  </si>
+  <si>
+    <t>Đặt tên 
+biến đầu tiên</t>
+  </si>
+  <si>
+    <t>=&gt;</t>
+  </si>
+  <si>
+    <t>$flag = true; ($n1 là sô, $n2 là số) thì echo Kết quả 2 + 2 = 4</t>
+  </si>
+  <si>
+    <t>$flag   = false; ($n1, $n2 không là số) thì echo Kết quả "Không thực hiện được"</t>
+  </si>
+  <si>
+    <t>&lt;div class = "result"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;img src = "images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;?php echo $image; ?&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.jpg" alt = "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;?php echo $image;?&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>$image = Aquarius</t>
+  </si>
+  <si>
+    <t>$name = Bảo Bình</t>
+  </si>
+  <si>
+    <t>$time = 20/1 - 19/2</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;img src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"images/Aquarius.jpg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" src="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Aquarius</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    &lt;p&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;?php echo $name;?&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(&lt;?php echo $image?&gt; : &lt;?php echo $time;?&gt;)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;p&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Bảo Bình</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;span&gt;(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Aquarius</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20/1 - 19/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>        &lt;div class="result"&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;img src="images/taurus.jpg" src="taurus" /&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;p&gt;Cung Bảo Bình &lt;span&gt;(Aquarius - 20/1 - 19/2)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;?php }?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;?php {?&gt;</t>
+  </si>
+  <si>
+    <t>C1:</t>
+  </si>
+  <si>
+    <t>             * Capricorn    23/12 - 19/01   Ma kết</t>
+  </si>
+  <si>
+    <t>             * Aquarius     20/01 - 19/02   Bảo Bình</t>
+  </si>
+  <si>
+    <t>             * Pisces       20/02 - 21/03   Song Ngư</t>
+  </si>
+  <si>
+    <t>             * Aries        22/03 - 20/04   Bạch Dương</t>
+  </si>
+  <si>
+    <t>             * Taurus       21/04 - 21/05   Kim Ngưu</t>
+  </si>
+  <si>
+    <t>             * Gemini       22/05 - 22/06   Song Tử</t>
+  </si>
+  <si>
+    <t>             * Cancer       23/06 - 23/07   Cự Giải</t>
+  </si>
+  <si>
+    <t>             * Leo          24/07 - 23/08   Sư Tử</t>
+  </si>
+  <si>
+    <t>             * Virgo        24/08 - 23/09   Xử Nữ</t>
+  </si>
+  <si>
+    <t>             * Libra        24/09 - 23/10   Thiên Xứng</t>
+  </si>
+  <si>
+    <t>             * Scorpio      24/10 - 22/11   Hổ Cáp</t>
+  </si>
+  <si>
+    <t>             * Sagittarius  23/11 - 22/12   Nhân Mã</t>
+  </si>
+  <si>
+    <t>        &lt;/div&gt;;</t>
+  </si>
+  <si>
+    <t>    '</t>
+  </si>
+  <si>
+    <t>&lt;?php </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>   &lt;div class="result"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;img src="images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' . $image . '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.jpg" alt="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' . $image . '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            &lt;p&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' . $name . '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(' . $image . '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>' . $time . '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>C2:</t>
+  </si>
+  <si>
+    <t>$image = abc</t>
+  </si>
+  <si>
+    <t>ucfirst ($image) = Abc</t>
+  </si>
+  <si>
+    <t>        echo $i . "&lt;br /&gt;";</t>
+  </si>
+  <si>
+    <t>For Loop</t>
+  </si>
+  <si>
+    <t>3 …</t>
+  </si>
+  <si>
+    <t>    for($i = 0; $i &lt;= 10;  $i++) {</t>
+  </si>
+  <si>
+    <t>    $i = 1;</t>
+  </si>
+  <si>
+    <t>    while ($i &lt;= 10) {</t>
+  </si>
+  <si>
+    <t>        $i++;</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>str_repeat("*",3);</t>
+  </si>
+  <si>
+    <t>Có 2 loại Hàm trong PHP</t>
+  </si>
+  <si>
+    <t>- Nhóm nhàm được PHP tự định nghĩa</t>
+  </si>
+  <si>
+    <t>- Hàm do người dùng tự định nghĩa</t>
+  </si>
+  <si>
+    <t>Hàm người dùng</t>
+  </si>
+  <si>
+    <t>Hàm không tham số &amp; không có trả về</t>
+  </si>
+  <si>
+    <t>Sự trả về của hàm</t>
+  </si>
+  <si>
+    <t>Truyền tham số vào hàm</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Phân biệt biến toàn cục &amp; biến cục bộ</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Phân biệt tham chiếu &amp; tham trị</t>
+  </si>
+  <si>
+    <t>Tìm hiểu include &amp; require</t>
+  </si>
+  <si>
+    <t>Xây dựng hàm vẽ các box</t>
+  </si>
+  <si>
+    <t>Lưu ý về cách đặt tên hàm</t>
+  </si>
+  <si>
+    <t>Biết cách khai báo &amp; gọi hàm không có tham số &amp; không có trả về.</t>
+  </si>
+  <si>
+    <t>function TênHàm () {}</t>
+  </si>
+  <si>
+    <t>Trong File HTML</t>
+  </si>
+  <si>
+    <t>&lt;body&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;div class = "content"&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;div style="width: 200px; height: 50px;"&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;p&gt;Box A&lt;span&gt;(300x200)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/body&gt;</t>
+  </si>
+  <si>
+    <t>Trong File PHP</t>
+  </si>
+  <si>
+    <t>            </t>
+  </si>
+  <si>
+    <t>    &lt;?php</t>
+  </si>
+  <si>
+    <t>        function createBox() {</t>
+  </si>
+  <si>
+    <t>        createBox();</t>
+  </si>
+  <si>
+    <t>        ?&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>            echo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;div style="width: 200px; height: 50px;"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            echo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;p&gt;Box A&lt;span&gt;(300x200)&lt;/span&gt;&lt;/p&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            echo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;/div&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>- Xây dựng hàm vẽ các box với sự trả về của hàm return</t>
+  </si>
+  <si>
+    <t>- Hàm trả về 1 giá trị</t>
+  </si>
+  <si>
+    <t>- Hàm trả về nhiều giá trị</t>
+  </si>
+  <si>
+    <t>- Hàm trả về giá trị True hoặc False</t>
+  </si>
+  <si>
+    <t>            $value = '&lt;div style="width: 200px; height: 50px;"&gt;';</t>
+  </si>
+  <si>
+    <t>            $value .= '&lt;p&gt;Box A&lt;span&gt;(300x200)&lt;/span&gt;&lt;/p&gt;'; </t>
+  </si>
+  <si>
+    <t>            $value .= '&lt;/div&gt;';</t>
+  </si>
+  <si>
+    <t>            return $value;</t>
+  </si>
+  <si>
+    <t>        $result = createBox();</t>
+  </si>
+  <si>
+    <t>        echo $result;</t>
+  </si>
+  <si>
+    <t>        function checkNumber() {</t>
+  </si>
+  <si>
+    <t>            $value = 13;</t>
+  </si>
+  <si>
+    <t>            if($value % 2 == 0) {</t>
+  </si>
+  <si>
+    <t>                return true;</t>
+  </si>
+  <si>
+    <t>            } else {</t>
+  </si>
+  <si>
+    <t>                return false;</t>
+  </si>
+  <si>
+    <t>        $result = checkNumber();</t>
+  </si>
+  <si>
+    <t>        if ($result == true) {</t>
+  </si>
+  <si>
+    <t>            echo "Số chẵn";</t>
+  </si>
+  <si>
+    <t>        }else {</t>
+  </si>
+  <si>
+    <t>            echo "Số lẻ";</t>
+  </si>
+  <si>
+    <t>- Hàm trả về giá trị True or False</t>
+  </si>
+  <si>
+    <t>TRUYỀN THAM số vào hàm</t>
+  </si>
+  <si>
+    <t>- Truyền nội dung vào cho box (Hàm 1 tham sô)</t>
+  </si>
+  <si>
+    <t>- Truyền chiều rộng, cao của box ( Hàm nhiều tham số)</t>
+  </si>
+  <si>
+    <t>- Ghán giá trị mặc định cho tham số</t>
+  </si>
+  <si>
+    <t>truyền tham số vào hàm</t>
+  </si>
+  <si>
+    <t>            echo $value . "&lt;br /&gt;";</t>
+  </si>
+  <si>
+    <r>
+      <t>        function checkNumber(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        $result = checkNumber(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>        function createBox($content) {</t>
+  </si>
+  <si>
+    <t>            $result = '&lt;div style="width: 200px; height: 50px;"&gt;';</t>
+  </si>
+  <si>
+    <t>            $result .= '&lt;p&gt;'.$content.'&lt;span&gt;(300x200)&lt;/span&gt;&lt;/p&gt;'; </t>
+  </si>
+  <si>
+    <t>            $result .= '&lt;/div&gt;';</t>
+  </si>
+  <si>
+    <t>            return $result;</t>
+  </si>
+  <si>
+    <t>        $boxA = createBox("Box A");</t>
+  </si>
+  <si>
+    <t>        $BoxB = createBox("Box B");</t>
+  </si>
+  <si>
+    <r>
+      <t>            $result .= '&lt;p&gt;'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.$content.'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;span&gt;(300x200)&lt;/span&gt;&lt;/p&gt;'; </t>
+    </r>
+  </si>
+  <si>
+    <t>            $result = '&lt;div style="width: '.$width.'px; height: 50px;"&gt;';</t>
+  </si>
+  <si>
+    <r>
+      <t>        function createBox($content,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        $boxA = createBox("Box A",</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        function createBox($content,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$width = 550</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; width Box B = 550px</t>
+  </si>
+  <si>
+    <t>-Phân biệt biến toàn cục (Global) &amp; biến cục bộ (Local)</t>
+  </si>
+  <si>
+    <t>            echo $boxA . $BoxB;</t>
+  </si>
+  <si>
+    <t>=&gt; width Box A = 500px</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +2102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1123,12 +2187,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1184,6 +2378,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1200,19 +2423,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1235,6 +2449,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1296,7 +2555,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1331,7 +2590,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1728,6 +2987,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
@@ -2277,12 +3556,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
       <c r="F27" s="7" t="s">
         <v>41</v>
       </c>
@@ -2291,34 +3570,34 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="24"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="7" t="s">
         <v>41</v>
       </c>
@@ -2328,10 +3607,10 @@
       <c r="F30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="24"/>
+      <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
@@ -2371,21 +3650,21 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="15" t="s">
         <v>41</v>
       </c>
@@ -2717,19 +3996,19 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="37" t="s">
         <v>143</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="38" t="s">
         <v>155</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="38" t="s">
         <v>161</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -2737,213 +4016,213 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="26"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K8" s="26"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="26"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K10" s="26"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="K11" s="26"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="22"/>
-      <c r="E12" s="26"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="3"/>
-      <c r="K12" s="26"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="E13" s="37"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="22"/>
-      <c r="E14" s="26"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="3"/>
-      <c r="K14" s="26"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="26"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="K15" s="26"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="37" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="26"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="26"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="26"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K18" s="26"/>
+      <c r="K18" s="37"/>
       <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="26"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K19" s="26"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="26"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="26"/>
+      <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="18" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="22"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2961,10 +4240,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="K103" sqref="K103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,140 +4257,486 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I2" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="J2" s="35"/>
+      <c r="I2" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="45"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="45"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="36"/>
-      <c r="J17" s="37"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="45"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="45"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="47"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="B25" s="32" t="s">
+      <c r="A25" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="32" t="s">
+      <c r="A26" s="41"/>
+      <c r="B26" s="26" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="26" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C98" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="M98" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D99" s="26" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3125,10 +4750,312 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="N8" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="L18" s="51" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="L19" s="52"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="L20" s="52"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="L21" s="52"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="L22" s="52"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="L23" s="52"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="L24" s="53"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="48" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="49"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="49"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L26:L29"/>
+    <mergeCell ref="L18:L24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +5063,7 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3144,27 +5071,1615 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>167</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="F15:F21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>310</v>
+      </c>
+      <c r="D16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>312</v>
+      </c>
+      <c r="D17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="56"/>
+      <c r="J23" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="56"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="59"/>
+      <c r="J24" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="59"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
+      <c r="J25" s="63" t="s">
+        <v>328</v>
+      </c>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="59"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="59"/>
+      <c r="J26" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="59"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="59"/>
+      <c r="J27" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="59"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
+      <c r="J28" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="59"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="62"/>
+      <c r="J29" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="59"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J30" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="59"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J31" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="59"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J32" s="63" t="s">
+        <v>330</v>
+      </c>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="59"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J33" s="63" t="s">
+        <v>331</v>
+      </c>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="59"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J34" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="59"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J35" s="60" t="s">
+        <v>325</v>
+      </c>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="62"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C38" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="56"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="59"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="59"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="J41" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="56"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="59"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="J42" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="59"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="59"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="J43" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="59"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="59"/>
+      <c r="J44" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="58"/>
+      <c r="R44" s="59"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="59"/>
+      <c r="J45" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
+      <c r="R45" s="59"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="59"/>
+      <c r="J46" s="57" t="s">
+        <v>342</v>
+      </c>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="59"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="59"/>
+      <c r="J47" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+      <c r="R47" s="59"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="64"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
+      <c r="J48" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+      <c r="R48" s="59"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B49" s="57" t="s">
+        <v>351</v>
+      </c>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="59"/>
+      <c r="J49" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="58"/>
+      <c r="R49" s="59"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="59"/>
+      <c r="J50" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="58"/>
+      <c r="R50" s="59"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="59"/>
+      <c r="J51" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="61"/>
+      <c r="O51" s="61"/>
+      <c r="P51" s="61"/>
+      <c r="Q51" s="61"/>
+      <c r="R51" s="62"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B52" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="59"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="58"/>
+      <c r="R52" s="58"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="59"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
+      <c r="P53" s="58"/>
+      <c r="Q53" s="58"/>
+      <c r="R53" s="58"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="59"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="64"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="59"/>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B56" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="62"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+      <c r="G8" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="56"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="G9" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="59"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="G10" s="57" t="s">
+        <v>366</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="59"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="G11" s="57" t="s">
+        <v>372</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="59"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="G12" s="57" t="s">
+        <v>368</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="59"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="G13" s="57" t="s">
+        <v>369</v>
+      </c>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="59"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
+      <c r="G14" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="59"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="G15" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="59"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
+      <c r="G16" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="59"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="64"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="G17" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
+        <v>364</v>
+      </c>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="G18" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="59"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="59"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="G20" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="59"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>354</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="G21" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="59"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="62"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="64"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
+      <c r="L29" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="56"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="59"/>
+      <c r="L30" s="57" t="s">
+        <v>376</v>
+      </c>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="59"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="59"/>
+      <c r="L31" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="59"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
+        <v>367</v>
+      </c>
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="59"/>
+      <c r="L32" s="57" t="s">
+        <v>367</v>
+      </c>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="58"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="59"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="57" t="s">
+        <v>368</v>
+      </c>
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="59"/>
+      <c r="L33" s="57" t="s">
+        <v>368</v>
+      </c>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="58"/>
+      <c r="T33" s="58"/>
+      <c r="U33" s="59"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="57" t="s">
+        <v>369</v>
+      </c>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="59"/>
+      <c r="L34" s="57" t="s">
+        <v>369</v>
+      </c>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
+      <c r="T34" s="58"/>
+      <c r="U34" s="59"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="59"/>
+      <c r="L35" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="58"/>
+      <c r="T35" s="58"/>
+      <c r="U35" s="59"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="59"/>
+      <c r="L36" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="58"/>
+      <c r="T36" s="58"/>
+      <c r="U36" s="59"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="59"/>
+      <c r="L37" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="68" t="s">
+        <v>380</v>
+      </c>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="59"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B38" s="58"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="59"/>
+      <c r="L38" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
+      <c r="S38" s="58"/>
+      <c r="T38" s="58"/>
+      <c r="U38" s="59"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B39" s="58"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="59"/>
+      <c r="L39" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="68" t="s">
+        <v>377</v>
+      </c>
+      <c r="R39" s="58"/>
+      <c r="S39" s="58"/>
+      <c r="T39" s="58"/>
+      <c r="U39" s="59"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="57"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="59"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
+      <c r="S40" s="58"/>
+      <c r="T40" s="58"/>
+      <c r="U40" s="59"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="59"/>
+      <c r="L41" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="M41" s="58"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="58"/>
+      <c r="R41" s="58"/>
+      <c r="S41" s="58"/>
+      <c r="T41" s="58"/>
+      <c r="U41" s="59"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="62"/>
+      <c r="L42" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="M42" s="61"/>
+      <c r="N42" s="61"/>
+      <c r="O42" s="61"/>
+      <c r="P42" s="61"/>
+      <c r="Q42" s="61"/>
+      <c r="R42" s="61"/>
+      <c r="S42" s="61"/>
+      <c r="T42" s="61"/>
+      <c r="U42" s="62"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Ch02 PHP ASNT 04:35 PM 20/06/2020
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/PHP.xlsx
+++ b/PHP-Course/BackEnd-PHP/PHP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PHP" sheetId="3" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="391">
   <si>
     <t>*</t>
   </si>
@@ -2028,6 +2028,36 @@
   </si>
   <si>
     <t>=&gt; width Box A = 500px</t>
+  </si>
+  <si>
+    <t>- Local: Là các biến được khai báo trong hàm &amp; và chỉ có thể được truy cập trong hàm đó. Biến cục bộ được xóa sau khi hàm của nó được thực thi xong.</t>
+  </si>
+  <si>
+    <t>- Global: Là các biến được khai báo bên ngoài tất cả các hàm. Được sử dụng tại bất kỳ vị trí nào trong chương trình.</t>
+  </si>
+  <si>
+    <t>Cách truy cập biến Global trong 1 hàm:</t>
+  </si>
+  <si>
+    <t>        $value = "ABC";</t>
+  </si>
+  <si>
+    <t>            global $value;</t>
+  </si>
+  <si>
+    <t>            echo $value;</t>
+  </si>
+  <si>
+    <t>            echo $boxA;</t>
+  </si>
+  <si>
+    <t>Khai báo trước return $result</t>
+  </si>
+  <si>
+    <t>            echo $GLOBALS["value"];</t>
+  </si>
+  <si>
+    <t>-Phân biệt tham chiếu &amp; tham trị</t>
   </si>
 </sst>
 </file>
@@ -2322,7 +2352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2407,6 +2437,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2467,33 +2524,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2989,20 +3037,451 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>378</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D6" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
+      <c r="K7" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="36"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
+      <c r="K8" s="37" t="s">
+        <v>384</v>
+      </c>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="39"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
+      <c r="K9" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="39"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="K10" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="39"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
+      <c r="K11" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="39"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
+      <c r="K12" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="39"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="39"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>385</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="69" t="s">
+        <v>388</v>
+      </c>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="K14" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="39"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>386</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="69" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q15" s="70"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="39"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="K16" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="39"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="39"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="K18" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="39"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="K19" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="39"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="K20" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="39"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="42"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K26" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E14:G15"/>
+    <mergeCell ref="P15:R16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3556,12 +4035,12 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="7" t="s">
         <v>41</v>
       </c>
@@ -3570,34 +4049,34 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="35"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="7" t="s">
         <v>41</v>
       </c>
@@ -3607,10 +4086,10 @@
       <c r="F30" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="35"/>
+      <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
@@ -3650,21 +4129,21 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="34"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="15" t="s">
         <v>41</v>
       </c>
@@ -3996,19 +4475,19 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="52" t="s">
         <v>143</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="53" t="s">
         <v>155</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="53" t="s">
         <v>161</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -4016,54 +4495,54 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="52"/>
       <c r="L8" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="52"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="52"/>
       <c r="L10" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="52"/>
       <c r="L11" s="3" t="s">
         <v>159</v>
       </c>
@@ -4071,9 +4550,9 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="22"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="3"/>
-      <c r="K12" s="37"/>
+      <c r="K12" s="52"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4081,148 +4560,148 @@
       <c r="B13" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="K13" s="37"/>
+      <c r="E13" s="52"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="22"/>
-      <c r="E14" s="37"/>
+      <c r="E14" s="52"/>
       <c r="F14" s="3"/>
-      <c r="K14" s="37"/>
+      <c r="K14" s="52"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="37"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="K15" s="37"/>
+      <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="52" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K16" s="37"/>
+      <c r="K16" s="52"/>
       <c r="L16" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="37"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="K18" s="37"/>
+      <c r="K18" s="52"/>
       <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="K19" s="37"/>
+      <c r="K19" s="52"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="52"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="18" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="22"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4257,124 +4736,124 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="J2" s="43"/>
+      <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="60"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="60"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="60"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="60"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="45"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="60"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="60"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="60"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I15" s="44"/>
-      <c r="J15" s="45"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="60"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="60"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="60"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="60"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="46"/>
-      <c r="J20" s="47"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -4382,13 +4861,13 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="26" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="26" t="s">
         <v>192</v>
       </c>
@@ -4880,7 +5359,7 @@
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
       <c r="J18" s="29"/>
-      <c r="L18" s="51" t="s">
+      <c r="L18" s="66" t="s">
         <v>272</v>
       </c>
     </row>
@@ -4897,7 +5376,7 @@
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
       <c r="J19" s="29"/>
-      <c r="L19" s="52"/>
+      <c r="L19" s="67"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
@@ -4912,7 +5391,7 @@
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
-      <c r="L20" s="52"/>
+      <c r="L20" s="67"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
@@ -4927,7 +5406,7 @@
       <c r="H21" s="29"/>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
-      <c r="L21" s="52"/>
+      <c r="L21" s="67"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
@@ -4942,7 +5421,7 @@
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
-      <c r="L22" s="52"/>
+      <c r="L22" s="67"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
@@ -4957,7 +5436,7 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
-      <c r="L23" s="52"/>
+      <c r="L23" s="67"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
@@ -4972,7 +5451,7 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
       <c r="J24" s="29"/>
-      <c r="L24" s="53"/>
+      <c r="L24" s="68"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -4989,7 +5468,7 @@
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
       <c r="K26" s="29"/>
-      <c r="L26" s="48" t="s">
+      <c r="L26" s="63" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5007,7 +5486,7 @@
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
-      <c r="L27" s="49"/>
+      <c r="L27" s="64"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
@@ -5023,7 +5502,7 @@
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
-      <c r="L28" s="49"/>
+      <c r="L28" s="64"/>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
@@ -5039,7 +5518,7 @@
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="50"/>
+      <c r="L29" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5100,7 +5579,7 @@
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="51" t="s">
+      <c r="F8" s="66" t="s">
         <v>295</v>
       </c>
       <c r="G8" s="2">
@@ -5115,7 +5594,7 @@
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="52"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="2">
         <v>1</v>
       </c>
@@ -5128,7 +5607,7 @@
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="52"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="2">
         <v>2</v>
       </c>
@@ -5141,7 +5620,7 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="52"/>
+      <c r="F11" s="67"/>
       <c r="G11" s="2" t="s">
         <v>296</v>
       </c>
@@ -5154,7 +5633,7 @@
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="53"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="2">
         <v>10</v>
       </c>
@@ -5168,7 +5647,7 @@
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="66" t="s">
         <v>295</v>
       </c>
       <c r="G15" s="2">
@@ -5183,7 +5662,7 @@
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="52"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="2">
         <v>1</v>
       </c>
@@ -5196,7 +5675,7 @@
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="52"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="2">
         <v>2</v>
       </c>
@@ -5209,7 +5688,7 @@
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" s="32"/>
-      <c r="F18" s="52"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="2">
         <v>3</v>
       </c>
@@ -5222,7 +5701,7 @@
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="32"/>
-      <c r="F19" s="52"/>
+      <c r="F19" s="67"/>
       <c r="G19" s="33" t="s">
         <v>301</v>
       </c>
@@ -5235,7 +5714,7 @@
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="52"/>
+      <c r="F20" s="67"/>
       <c r="G20" s="33" t="s">
         <v>301</v>
       </c>
@@ -5248,7 +5727,7 @@
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="53"/>
+      <c r="F21" s="68"/>
       <c r="G21" s="2">
         <v>10</v>
       </c>
@@ -5271,7 +5750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
@@ -5412,223 +5891,223 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
-      <c r="J23" s="54" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="J23" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="56"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="36"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="37" t="s">
         <v>321</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="59"/>
-      <c r="J24" s="57" t="s">
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
+      <c r="J24" s="37" t="s">
         <v>321</v>
       </c>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="59"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="39"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="59"/>
-      <c r="J25" s="63" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+      <c r="J25" s="43" t="s">
         <v>328</v>
       </c>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="59"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-      <c r="J26" s="57" t="s">
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
+      <c r="J26" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="59"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="39"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="57" t="s">
+      <c r="B27" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
-      <c r="J27" s="57" t="s">
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
+      <c r="J27" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="59"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="39"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="59"/>
-      <c r="J28" s="57" t="s">
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+      <c r="J28" s="37" t="s">
         <v>333</v>
       </c>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="59"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="39"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
-      <c r="J29" s="57" t="s">
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="J29" s="37" t="s">
         <v>334</v>
       </c>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="59"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="39"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="57" t="s">
+      <c r="J30" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="59"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="39"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="57" t="s">
+      <c r="J31" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="59"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="39"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="63" t="s">
+      <c r="J32" s="43" t="s">
         <v>330</v>
       </c>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="59"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="39"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J33" s="63" t="s">
+      <c r="J33" s="43" t="s">
         <v>331</v>
       </c>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="59"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="39"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J34" s="57" t="s">
+      <c r="J34" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="59"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="39"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="60" t="s">
+      <c r="J35" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
-      <c r="P35" s="61"/>
-      <c r="Q35" s="62"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="42"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C38" s="13" t="s">
@@ -5639,311 +6118,311 @@
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="59"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="58"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="39"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="37" t="s">
         <v>346</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="59"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-      <c r="J41" s="54" t="s">
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="39"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="J41" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="K41" s="55"/>
-      <c r="L41" s="55"/>
-      <c r="M41" s="55"/>
-      <c r="N41" s="55"/>
-      <c r="O41" s="55"/>
-      <c r="P41" s="55"/>
-      <c r="Q41" s="55"/>
-      <c r="R41" s="56"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="36"/>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="37" t="s">
         <v>347</v>
       </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="59"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="J42" s="57" t="s">
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="39"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="J42" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="59"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="39"/>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B43" s="57" t="s">
+      <c r="B43" s="37" t="s">
         <v>348</v>
       </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="J43" s="57" t="s">
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="39"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="J43" s="37" t="s">
         <v>339</v>
       </c>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="59"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="39"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="59"/>
-      <c r="J44" s="57" t="s">
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
+      <c r="J44" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="K44" s="58"/>
-      <c r="L44" s="58"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="58"/>
-      <c r="O44" s="58"/>
-      <c r="P44" s="58"/>
-      <c r="Q44" s="58"/>
-      <c r="R44" s="59"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="39"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="59"/>
-      <c r="J45" s="57" t="s">
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="39"/>
+      <c r="J45" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-      <c r="P45" s="58"/>
-      <c r="Q45" s="58"/>
-      <c r="R45" s="59"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="39"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="57" t="s">
+      <c r="B46" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="59"/>
-      <c r="J46" s="57" t="s">
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="39"/>
+      <c r="J46" s="37" t="s">
         <v>342</v>
       </c>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
-      <c r="M46" s="58"/>
-      <c r="N46" s="58"/>
-      <c r="O46" s="58"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="58"/>
-      <c r="R46" s="59"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="39"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="59"/>
-      <c r="J47" s="57" t="s">
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="39"/>
+      <c r="J47" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
-      <c r="P47" s="58"/>
-      <c r="Q47" s="58"/>
-      <c r="R47" s="59"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38"/>
+      <c r="N47" s="38"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="39"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B48" s="64"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="59"/>
-      <c r="J48" s="57" t="s">
+      <c r="B48" s="44"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
+      <c r="J48" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
-      <c r="M48" s="58"/>
-      <c r="N48" s="58"/>
-      <c r="O48" s="58"/>
-      <c r="P48" s="58"/>
-      <c r="Q48" s="58"/>
-      <c r="R48" s="59"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38"/>
+      <c r="N48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="39"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="37" t="s">
         <v>351</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="59"/>
-      <c r="J49" s="57" t="s">
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
+      <c r="J49" s="37" t="s">
         <v>343</v>
       </c>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
-      <c r="M49" s="58"/>
-      <c r="N49" s="58"/>
-      <c r="O49" s="58"/>
-      <c r="P49" s="58"/>
-      <c r="Q49" s="58"/>
-      <c r="R49" s="59"/>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="39"/>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="59"/>
-      <c r="J50" s="57" t="s">
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
+      <c r="J50" s="37" t="s">
         <v>344</v>
       </c>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="58"/>
-      <c r="P50" s="58"/>
-      <c r="Q50" s="58"/>
-      <c r="R50" s="59"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38"/>
+      <c r="R50" s="39"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="59"/>
-      <c r="J51" s="60" t="s">
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="39"/>
+      <c r="J51" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="K51" s="61"/>
-      <c r="L51" s="61"/>
-      <c r="M51" s="61"/>
-      <c r="N51" s="61"/>
-      <c r="O51" s="61"/>
-      <c r="P51" s="61"/>
-      <c r="Q51" s="61"/>
-      <c r="R51" s="62"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="41"/>
+      <c r="P51" s="41"/>
+      <c r="Q51" s="41"/>
+      <c r="R51" s="42"/>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="59"/>
-      <c r="J52" s="66"/>
-      <c r="K52" s="58"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="58"/>
-      <c r="N52" s="58"/>
-      <c r="O52" s="58"/>
-      <c r="P52" s="58"/>
-      <c r="Q52" s="58"/>
-      <c r="R52" s="58"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="39"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="37" t="s">
         <v>355</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="59"/>
-      <c r="J53" s="66"/>
-      <c r="K53" s="58"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="58"/>
-      <c r="N53" s="58"/>
-      <c r="O53" s="58"/>
-      <c r="P53" s="58"/>
-      <c r="Q53" s="58"/>
-      <c r="R53" s="58"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="39"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="38"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="38"/>
+      <c r="R53" s="38"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="57" t="s">
+      <c r="B54" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="59"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="39"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="64"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="59"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="60" t="s">
+      <c r="B56" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="62"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5956,8 +6435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5991,323 +6470,323 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="G8" s="54" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="G8" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="56"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
-      <c r="G9" s="57" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+      <c r="G9" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="39"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="37" t="s">
         <v>362</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="G10" s="57" t="s">
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
+      <c r="G10" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="37" t="s">
         <v>347</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="G11" s="57" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="G11" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="59"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="39"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="37" t="s">
         <v>348</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="G12" s="57" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="G12" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="59"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="G13" s="57" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="G13" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="59"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="39"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-      <c r="G14" s="57" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="G14" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="59"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="G15" s="57" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="G15" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="59"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
       <c r="G16" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="59"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
       <c r="G17" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="59"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
       <c r="G18" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="59"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="59"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
-      <c r="G20" s="57" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="G20" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="59"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="39"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="G21" s="57" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="G21" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="59"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="39"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="37" t="s">
         <v>355</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="59"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="62"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="42"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="62"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
@@ -6318,365 +6797,365 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="56"/>
-      <c r="L29" s="54" t="s">
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36"/>
+      <c r="L29" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="55"/>
-      <c r="U29" s="56"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="35"/>
+      <c r="T29" s="35"/>
+      <c r="U29" s="36"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="59"/>
-      <c r="L30" s="57" t="s">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
+      <c r="L30" s="37" t="s">
         <v>376</v>
       </c>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="59"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="39"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="59"/>
-      <c r="L31" s="57" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="L31" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="59"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
+      <c r="S31" s="38"/>
+      <c r="T31" s="38"/>
+      <c r="U31" s="39"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="59"/>
-      <c r="L32" s="57" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39"/>
+      <c r="L32" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="59"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="38"/>
+      <c r="T32" s="38"/>
+      <c r="U32" s="39"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="59"/>
-      <c r="L33" s="57" t="s">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="L33" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
-      <c r="T33" s="58"/>
-      <c r="U33" s="59"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="38"/>
+      <c r="U33" s="39"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="59"/>
-      <c r="L34" s="57" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="39"/>
+      <c r="L34" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="59"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
+      <c r="T34" s="38"/>
+      <c r="U34" s="39"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="59"/>
-      <c r="L35" s="57" t="s">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="39"/>
+      <c r="L35" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
-      <c r="T35" s="58"/>
-      <c r="U35" s="59"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="38"/>
+      <c r="U35" s="39"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="59"/>
-      <c r="L36" s="57" t="s">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
+      <c r="L36" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="58"/>
-      <c r="T36" s="58"/>
-      <c r="U36" s="59"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="38"/>
+      <c r="T36" s="38"/>
+      <c r="U36" s="39"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="59"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
       <c r="L37" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="68" t="s">
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="48" t="s">
         <v>380</v>
       </c>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="59"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
+      <c r="T37" s="38"/>
+      <c r="U37" s="39"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="59"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
       <c r="L38" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="58"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="58"/>
-      <c r="R38" s="58"/>
-      <c r="S38" s="58"/>
-      <c r="T38" s="58"/>
-      <c r="U38" s="59"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38"/>
+      <c r="R38" s="38"/>
+      <c r="S38" s="38"/>
+      <c r="T38" s="38"/>
+      <c r="U38" s="39"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="59"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
       <c r="L39" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="68" t="s">
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="48" t="s">
         <v>377</v>
       </c>
-      <c r="R39" s="58"/>
-      <c r="S39" s="58"/>
-      <c r="T39" s="58"/>
-      <c r="U39" s="59"/>
+      <c r="R39" s="38"/>
+      <c r="S39" s="38"/>
+      <c r="T39" s="38"/>
+      <c r="U39" s="39"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="59"/>
-      <c r="L40" s="57"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="58"/>
-      <c r="S40" s="58"/>
-      <c r="T40" s="58"/>
-      <c r="U40" s="59"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
+      <c r="T40" s="38"/>
+      <c r="U40" s="39"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="59"/>
-      <c r="L41" s="57" t="s">
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
+      <c r="L41" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="58"/>
-      <c r="R41" s="58"/>
-      <c r="S41" s="58"/>
-      <c r="T41" s="58"/>
-      <c r="U41" s="59"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
+      <c r="T41" s="38"/>
+      <c r="U41" s="39"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="62"/>
-      <c r="L42" s="60" t="s">
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="42"/>
+      <c r="L42" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="M42" s="61"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="61"/>
-      <c r="P42" s="61"/>
-      <c r="Q42" s="61"/>
-      <c r="R42" s="61"/>
-      <c r="S42" s="61"/>
-      <c r="T42" s="61"/>
-      <c r="U42" s="62"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>